<commit_message>
changed data and reworked some mistakes in processing
</commit_message>
<xml_diff>
--- a/clear_data/men_2015_2022.xlsx
+++ b/clear_data/men_2015_2022.xlsx
@@ -466,28 +466,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>56648154</v>
+        <v>67771723</v>
       </c>
       <c r="C2" t="n">
-        <v>57300499</v>
+        <v>67896547</v>
       </c>
       <c r="D2" t="n">
-        <v>58016625</v>
+        <v>68044296</v>
       </c>
       <c r="E2" t="n">
-        <v>58718314</v>
+        <v>68119911</v>
       </c>
       <c r="F2" t="n">
-        <v>59255244</v>
+        <v>68096423</v>
       </c>
       <c r="G2" t="n">
-        <v>59785997</v>
+        <v>68123067</v>
       </c>
       <c r="H2" t="n">
-        <v>60000609</v>
+        <v>67847796</v>
       </c>
       <c r="I2" t="n">
-        <v>60104958</v>
+        <v>67654279</v>
       </c>
     </row>
     <row r="3">
@@ -497,28 +497,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>15052384</v>
+        <v>17865082</v>
       </c>
       <c r="C3" t="n">
-        <v>15269975</v>
+        <v>17939648</v>
       </c>
       <c r="D3" t="n">
-        <v>15484678</v>
+        <v>17998603</v>
       </c>
       <c r="E3" t="n">
-        <v>15714841</v>
+        <v>18059917</v>
       </c>
       <c r="F3" t="n">
-        <v>15906325</v>
+        <v>18099311</v>
       </c>
       <c r="G3" t="n">
-        <v>16085435</v>
+        <v>18139809</v>
       </c>
       <c r="H3" t="n">
-        <v>16146083</v>
+        <v>18055158</v>
       </c>
       <c r="I3" t="n">
-        <v>16188232</v>
+        <v>18013939</v>
       </c>
     </row>
     <row r="4">
@@ -528,28 +528,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5301129</v>
+        <v>6389901</v>
       </c>
       <c r="C4" t="n">
-        <v>5359917</v>
+        <v>6381639</v>
       </c>
       <c r="D4" t="n">
-        <v>5442416</v>
+        <v>6404542</v>
       </c>
       <c r="E4" t="n">
-        <v>5532755</v>
+        <v>6434640</v>
       </c>
       <c r="F4" t="n">
-        <v>5603116</v>
+        <v>6444785</v>
       </c>
       <c r="G4" t="n">
-        <v>5667916</v>
+        <v>6449822</v>
       </c>
       <c r="H4" t="n">
-        <v>5701777</v>
+        <v>6429482</v>
       </c>
       <c r="I4" t="n">
-        <v>5724851</v>
+        <v>6416656</v>
       </c>
     </row>
     <row r="5">
@@ -559,10 +559,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5452707</v>
+        <v>6506418</v>
       </c>
       <c r="C5" t="n">
-        <v>5514767</v>
+        <v>6523269</v>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
@@ -580,22 +580,22 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>6511705.910000001</v>
+        <v>7624798.900000001</v>
       </c>
       <c r="E6" t="n">
-        <v>6586241.900000001</v>
+        <v>7634657.890000002</v>
       </c>
       <c r="F6" t="n">
-        <v>6651748.930000001</v>
+        <v>7643546.920000001</v>
       </c>
       <c r="G6" t="n">
-        <v>6714610.930000001</v>
+        <v>7652586.920000001</v>
       </c>
       <c r="H6" t="n">
-        <v>6770549.920000001</v>
+        <v>7661204.900000001</v>
       </c>
       <c r="I6" t="n">
-        <v>6789699.94</v>
+        <v>7646030.920000001</v>
       </c>
     </row>
     <row r="7">
@@ -605,28 +605,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3745202.930000001</v>
+        <v>4570466.920000001</v>
       </c>
       <c r="C7" t="n">
-        <v>3796198.900000001</v>
+        <v>4602546.880000002</v>
       </c>
       <c r="D7" t="n">
-        <v>3847672.95</v>
+        <v>4633054.930000001</v>
       </c>
       <c r="E7" t="n">
-        <v>3899059.920000001</v>
+        <v>4658936.920000001</v>
       </c>
       <c r="F7" t="n">
-        <v>3945656.94</v>
+        <v>4682831.920000001</v>
       </c>
       <c r="G7" t="n">
-        <v>4004016.96</v>
+        <v>4720031.94</v>
       </c>
       <c r="H7" t="n">
-        <v>4056384.930000001</v>
+        <v>4739727.920000001</v>
       </c>
       <c r="I7" t="n">
-        <v>4100418.95</v>
+        <v>4760139.94</v>
       </c>
     </row>
     <row r="8">
@@ -636,28 +636,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>11469245.93</v>
+        <v>13694958.92</v>
       </c>
       <c r="C8" t="n">
-        <v>11561265.9</v>
+        <v>13678443.9</v>
       </c>
       <c r="D8" t="n">
-        <v>11672350.89</v>
+        <v>13668366.89</v>
       </c>
       <c r="E8" t="n">
-        <v>11772873.93</v>
+        <v>13636054.93</v>
       </c>
       <c r="F8" t="n">
-        <v>11830586.9</v>
+        <v>13573442.9</v>
       </c>
       <c r="G8" t="n">
-        <v>11889812.92</v>
+        <v>13528662.9</v>
       </c>
       <c r="H8" t="n">
-        <v>11878978.93</v>
+        <v>13426671.92</v>
       </c>
       <c r="I8" t="n">
-        <v>11847098.9</v>
+        <v>13340651.9</v>
       </c>
     </row>
     <row r="9">
@@ -667,28 +667,28 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>4790006.950000001</v>
+        <v>5715802.940000001</v>
       </c>
       <c r="C9" t="n">
-        <v>4851858.890000002</v>
+        <v>5730861.880000002</v>
       </c>
       <c r="D9" t="n">
-        <v>4922105.930000002</v>
+        <v>5750735.930000002</v>
       </c>
       <c r="E9" t="n">
-        <v>4986661.920000001</v>
+        <v>5757597.910000001</v>
       </c>
       <c r="F9" t="n">
-        <v>5033084.910000001</v>
+        <v>5756688.890000002</v>
       </c>
       <c r="G9" t="n">
-        <v>5079482.94</v>
+        <v>5765302.930000001</v>
       </c>
       <c r="H9" t="n">
-        <v>5099756.930000001</v>
+        <v>5750443.920000001</v>
       </c>
       <c r="I9" t="n">
-        <v>5111190.910000001</v>
+        <v>5740710.900000001</v>
       </c>
     </row>
     <row r="10">
@@ -698,16 +698,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>7491620.920000001</v>
+        <v>8988287.92</v>
       </c>
       <c r="C10" t="n">
-        <v>7568089.920000001</v>
+        <v>8994098.91</v>
       </c>
       <c r="D10" t="n">
-        <v>7648410.940000001</v>
+        <v>8996035.940000001</v>
       </c>
       <c r="E10" t="n">
-        <v>7719114.94</v>
+        <v>8978336.93</v>
       </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
@@ -725,16 +725,16 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>6928862.930000001</v>
+        <v>7968701.910000001</v>
       </c>
       <c r="G11" t="n">
-        <v>6966749.920000002</v>
+        <v>7945532.900000002</v>
       </c>
       <c r="H11" t="n">
-        <v>6965906.910000001</v>
+        <v>7888370.900000001</v>
       </c>
       <c r="I11" t="n">
-        <v>6954738.920000002</v>
+        <v>7846112.920000002</v>
       </c>
     </row>
     <row r="12">
@@ -744,16 +744,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2455244.94</v>
+        <v>2985001.930000001</v>
       </c>
       <c r="C12" t="n">
-        <v>2468970.94</v>
+        <v>2974920.930000001</v>
       </c>
       <c r="D12" t="n">
-        <v>2487272.91</v>
+        <v>2968142.91</v>
       </c>
       <c r="E12" t="n">
-        <v>2506753.9</v>
+        <v>2959755.9</v>
       </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
@@ -771,16 +771,16 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>3355851.9</v>
+        <v>3927102.88</v>
       </c>
       <c r="G13" t="n">
-        <v>3377964.95</v>
+        <v>3921310.95</v>
       </c>
       <c r="H13" t="n">
-        <v>3381164.92</v>
+        <v>3896727.920000001</v>
       </c>
       <c r="I13" t="n">
-        <v>3388714.92</v>
+        <v>3890021.91</v>
       </c>
     </row>
     <row r="14">
@@ -790,10 +790,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>890587.96</v>
+        <v>1055776.95</v>
       </c>
       <c r="C14" t="n">
-        <v>909434.9399999999</v>
+        <v>1071096.94</v>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>

</xml_diff>